<commit_message>
Created, and Updated the pit Scouting sheet
</commit_message>
<xml_diff>
--- a/Pre-Season/Sheet Revisions/2019 pit scouting REV 5.xlsx
+++ b/Pre-Season/Sheet Revisions/2019 pit scouting REV 5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\team3641\2019\Scouting Laptop Github\2019Scouting\Pre-Season\Sheet Revisions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A9D8171-7EF3-4A7A-B8BF-D1DFE92621DB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EE306C-11A3-4916-AB0C-29021DA72899}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t>PIT SCOUTING</t>
   </si>
@@ -34,9 +34,6 @@
     <t>Place</t>
   </si>
   <si>
-    <t>How do you drive? (circle one)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Camera </t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>Hatch</t>
   </si>
   <si>
-    <t>Ball</t>
-  </si>
-  <si>
     <t>Right</t>
   </si>
   <si>
@@ -142,9 +136,6 @@
     <t xml:space="preserve">To which level?(circle one) </t>
   </si>
   <si>
-    <t>How?(have them explain how they climb)</t>
-  </si>
-  <si>
     <t>___________________________________________________________________________________________________________________________________________________________</t>
   </si>
   <si>
@@ -167,6 +158,12 @@
   </si>
   <si>
     <t xml:space="preserve">How many levels can you do on the rocket Hatch?(circle one) </t>
+  </si>
+  <si>
+    <t>How do you drive? (circle one if avaliable)</t>
+  </si>
+  <si>
+    <t>If so, How? (have them explain how they climb)</t>
   </si>
 </sst>
 </file>
@@ -593,7 +590,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -604,7 +601,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="24.6" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>0</v>
@@ -624,31 +621,31 @@
     </row>
     <row r="3" spans="1:12" ht="24.6" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>7</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="24.6" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -660,66 +657,66 @@
         <v>2</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="24.6" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="G5" s="6"/>
       <c r="I5" s="3"/>
       <c r="J5" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="24.6" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:12" ht="24.6" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -727,7 +724,7 @@
     </row>
     <row r="8" spans="1:12" ht="24.6" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -735,47 +732,47 @@
     </row>
     <row r="9" spans="1:12" ht="24.6" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="24.6" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="24.6" customHeight="1">
       <c r="A11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="24.6" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E12" s="6">
         <v>1</v>
@@ -787,7 +784,7 @@
         <v>3</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J12" s="6">
         <v>1</v>
@@ -801,56 +798,56 @@
     </row>
     <row r="13" spans="1:12" ht="24.6" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="24.6" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="24.6" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:12" ht="24.6" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="24.6" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="24.6" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="24.6" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G19" s="8"/>
     </row>
     <row r="20" spans="1:7" ht="24.6" customHeight="1">
       <c r="A20" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E20" s="6">
         <v>1</v>
@@ -864,33 +861,33 @@
     </row>
     <row r="21" spans="1:7" ht="24.6" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="24.6" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="24.6" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="24.6" customHeight="1">
       <c r="A24" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="24.6" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.6">
@@ -898,7 +895,7 @@
     </row>
     <row r="27" spans="1:7" ht="15.6">
       <c r="A27" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.6">
@@ -906,7 +903,7 @@
     </row>
     <row r="29" spans="1:7" ht="15.6">
       <c r="A29" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.6">

</xml_diff>